<commit_message>
finished wer cer calculation
</commit_message>
<xml_diff>
--- a/data/phoneticData.xlsx
+++ b/data/phoneticData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F1E09F-6402-4564-A71A-F4560EB4FD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FFAC73-0F99-4CDC-976D-DC5D7A7F65A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5817" uniqueCount="1373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5939" uniqueCount="1407">
   <si>
     <t>iso639_3</t>
   </si>
@@ -3977,9 +3977,6 @@
     <t>online</t>
   </si>
   <si>
-    <t>theNorthWindAndTheSun/alamblak.pdf</t>
-  </si>
-  <si>
     <t>theNorthWindAndTheSun/standard-chinese-beijing.pdf</t>
   </si>
   <si>
@@ -4164,6 +4161,111 @@
   </si>
   <si>
     <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/tur-orthographic.txt</t>
+  </si>
+  <si>
+    <t>alamblak.pdf</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun\pes-orthographic.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun\kor-orthographic.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun\hin-orthographic.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/cmn.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/deu-broad.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/deu-narrow.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/ell.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/eng-broad.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/eng-narrow.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/eus-broad.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/eus-narrow.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/heb.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/ind.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/kat-broad.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/mya.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/spa-broad.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/spa-narrow.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/tha.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/tur.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/hin.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/kor.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/pes.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/hin-orthographic.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/word-list/hin_deva_broad_filtered.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/kor-orthographic.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/word-list/kor_hang_narrow_filtered.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/pes-orthographic.txt</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/word-list/per_arab_broad.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/word-list/per_arab_narrow.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/word-list/gre_grek_narrow.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/masterThesis/data/word-list/hin_deva_narrow.tsv</t>
+  </si>
+  <si>
+    <t>C:\Users\debor\masterThesis\data\word-list\heb_hebr_narrow.tsv</t>
+  </si>
+  <si>
+    <t>C:\Users\debor\masterThesis\data\word-list\ind_latn_narrow.tsv</t>
+  </si>
+  <si>
+    <t>C:\Users\debor\masterThesis\data\word-list\tur_latn_narrow_filtered.tsv</t>
   </si>
 </sst>
 </file>
@@ -4646,7 +4748,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9:I465"/>
+      <selection pane="bottomLeft" activeCell="A251" sqref="A251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4776,7 +4878,7 @@
       <c r="W2" s="2"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -5057,7 +5159,7 @@
       <c r="W8" s="2"/>
       <c r="Y8" s="3"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -5071,13 +5173,13 @@
         <v>218</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>328</v>
@@ -5542,7 +5644,7 @@
         <v>218</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>1310</v>
+        <v>1372</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>5</v>
@@ -6012,10 +6114,10 @@
         <v>753</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>752</v>
@@ -6061,10 +6163,10 @@
         <v>753</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="J31" s="9" t="s">
         <v>752</v>
@@ -7769,13 +7871,13 @@
         <v>218</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="H71" s="9" t="s">
+        <v>1319</v>
+      </c>
+      <c r="I71" s="9" t="s">
         <v>1320</v>
-      </c>
-      <c r="I71" s="9" t="s">
-        <v>1321</v>
       </c>
       <c r="J71" s="13" t="s">
         <v>208</v>
@@ -8924,13 +9026,13 @@
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="9" t="s">
+        <v>1312</v>
+      </c>
+      <c r="I94" s="9" t="s">
         <v>1313</v>
       </c>
-      <c r="I94" s="9" t="s">
-        <v>1314</v>
-      </c>
       <c r="J94" s="9" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="K94" s="12">
         <v>44386</v>
@@ -8974,13 +9076,13 @@
       </c>
       <c r="G95" s="8"/>
       <c r="H95" s="9" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="K95" s="12">
         <v>44386</v>
@@ -9634,10 +9736,10 @@
         <v>754</v>
       </c>
       <c r="H110" s="9" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="I110" s="9" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="J110" s="9" t="s">
         <v>755</v>
@@ -12791,10 +12893,10 @@
         <v>739</v>
       </c>
       <c r="H186" s="9" t="s">
+        <v>1324</v>
+      </c>
+      <c r="I186" s="9" t="s">
         <v>1325</v>
-      </c>
-      <c r="I186" s="9" t="s">
-        <v>1326</v>
       </c>
       <c r="J186" s="9" t="s">
         <v>740</v>
@@ -12907,10 +13009,10 @@
         <v>751</v>
       </c>
       <c r="H189" s="9" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="I189" s="9" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="J189" s="9" t="s">
         <v>750</v>
@@ -12928,7 +13030,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
         <v>50</v>
       </c>
@@ -12947,8 +13049,11 @@
       <c r="G190" s="8" t="s">
         <v>745</v>
       </c>
+      <c r="H190" s="9" t="s">
+        <v>1375</v>
+      </c>
       <c r="I190" s="9" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="J190" s="9" t="s">
         <v>741</v>
@@ -14389,10 +14494,10 @@
         <v>737</v>
       </c>
       <c r="H230" s="9" t="s">
+        <v>1329</v>
+      </c>
+      <c r="I230" s="9" t="s">
         <v>1330</v>
-      </c>
-      <c r="I230" s="9" t="s">
-        <v>1331</v>
       </c>
       <c r="J230" s="9" t="s">
         <v>738</v>
@@ -14430,10 +14535,10 @@
         <v>737</v>
       </c>
       <c r="H231" s="9" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="I231" s="9" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="J231" s="9" t="s">
         <v>738</v>
@@ -15071,7 +15176,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="251" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
         <v>72</v>
       </c>
@@ -15087,8 +15192,11 @@
       <c r="G251" s="8" t="s">
         <v>748</v>
       </c>
+      <c r="H251" s="9" t="s">
+        <v>1374</v>
+      </c>
       <c r="I251" s="9" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="J251" s="13" t="s">
         <v>747</v>
@@ -17437,10 +17545,10 @@
         <v>735</v>
       </c>
       <c r="H319" s="9" t="s">
+        <v>1332</v>
+      </c>
+      <c r="I319" s="9" t="s">
         <v>1333</v>
-      </c>
-      <c r="I319" s="9" t="s">
-        <v>1334</v>
       </c>
       <c r="J319" s="13" t="s">
         <v>736</v>
@@ -19298,7 +19406,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="371" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A371" s="6" t="s">
         <v>184</v>
       </c>
@@ -19314,8 +19422,11 @@
       <c r="G371" s="8" t="s">
         <v>761</v>
       </c>
+      <c r="H371" s="9" t="s">
+        <v>1373</v>
+      </c>
       <c r="I371" s="9" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="J371" s="9" t="s">
         <v>760</v>
@@ -21144,10 +21255,10 @@
         <v>757</v>
       </c>
       <c r="H424" s="6" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="I424" s="9" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="J424" s="13" t="s">
         <v>756</v>
@@ -21188,10 +21299,10 @@
         <v>757</v>
       </c>
       <c r="H425" s="6" t="s">
+        <v>1336</v>
+      </c>
+      <c r="I425" s="9" t="s">
         <v>1337</v>
-      </c>
-      <c r="I425" s="9" t="s">
-        <v>1338</v>
       </c>
       <c r="J425" s="13" t="s">
         <v>756</v>
@@ -22282,10 +22393,10 @@
         <v>749</v>
       </c>
       <c r="H453" s="9" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="I453" s="9" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="J453" s="9" t="s">
         <v>746</v>
@@ -22685,10 +22796,10 @@
         <v>759</v>
       </c>
       <c r="H465" s="9" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="I465" s="9" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="J465" s="13" t="s">
         <v>758</v>
@@ -24067,12 +24178,10 @@
   <autoFilter ref="A1:P509" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="full text"/>
         <filter val="full text (the north wind and the sun)"/>
-        <filter val="full text, word list"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="7">
+    <filterColumn colId="8">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
@@ -24104,245 +24213,662 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5C2734-B933-4C84-90BB-81AC6BC51564}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1"/>
     <col min="3" max="3" width="70.140625" customWidth="1"/>
     <col min="4" max="4" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="C1" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1376</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C2" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1377</v>
+      </c>
+      <c r="E2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>1377</v>
+      </c>
+      <c r="E5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>1362</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C7" t="s">
         <v>1347</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="D7" s="9" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>1363</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
         <v>1348</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="D8" s="9" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B9" s="9" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E11" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>1364</v>
       </c>
-      <c r="C5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="C12" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>1364</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C13" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E14" t="s">
+        <v>219</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C15" t="s">
         <v>1350</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E15" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>1365</v>
       </c>
-      <c r="C7" t="s">
-        <v>1351</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="C16" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>1384</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>1365</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C17" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1384</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E20" t="s">
+        <v>219</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E23" t="s">
+        <v>243</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E25" t="s">
+        <v>243</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C26" t="s">
         <v>1352</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>1366</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1354</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>1367</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1355</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>1368</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1356</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>1369</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1357</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>1370</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1358</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>1370</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D26" s="9" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C27" t="s">
         <v>1359</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="D27" s="9" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>1371</v>
       </c>
-      <c r="C15" t="s">
-        <v>1353</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>1372</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1360</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>1341</v>
-      </c>
+      <c r="C28" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added WER CER table
</commit_message>
<xml_diff>
--- a/data/phoneticData.xlsx
+++ b/data/phoneticData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FFAC73-0F99-4CDC-976D-DC5D7A7F65A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9631F66-CED1-4C7F-AF92-65FDEDBCBAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5939" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5970" uniqueCount="1429">
   <si>
     <t>iso639_3</t>
   </si>
@@ -4091,12 +4091,6 @@
     <t>C:/Users/debor/wikipron/data/scrape/tsv/gre_grek_broad_filtered.tsv</t>
   </si>
   <si>
-    <t>C:/Users/debor/wikipron/data/scrape/tsv/eng_latn_uk_broad_filtered.tsv</t>
-  </si>
-  <si>
-    <t>C:/Users/debor/wikipron/data/scrape/tsv/eng_latn_uk_narrow.tsv</t>
-  </si>
-  <si>
     <t>C:/Users/debor/wikipron/data/scrape/tsv/baq_latn_broad.tsv</t>
   </si>
   <si>
@@ -4266,6 +4260,78 @@
   </si>
   <si>
     <t>C:\Users\debor\masterThesis\data\word-list\tur_latn_narrow_filtered.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/wikipron/data/scrape/tsv/eng_latn_us_broad_filtered.tsv</t>
+  </si>
+  <si>
+    <t>C:/Users/debor/wikipron/data/scrape/tsv/eng_latn_us_narrow.tsv</t>
+  </si>
+  <si>
+    <t>133\,686</t>
+  </si>
+  <si>
+    <t>34\,145</t>
+  </si>
+  <si>
+    <t>10\,984</t>
+  </si>
+  <si>
+    <t>10\,547</t>
+  </si>
+  <si>
+    <t>57\,230</t>
+  </si>
+  <si>
+    <t>1\,633</t>
+  </si>
+  <si>
+    <t>1\,742</t>
+  </si>
+  <si>
+    <t>1\,439</t>
+  </si>
+  <si>
+    <t>9\,563</t>
+  </si>
+  <si>
+    <t>10\,812</t>
+  </si>
+  <si>
+    <t>1\,555</t>
+  </si>
+  <si>
+    <t>2\,637</t>
+  </si>
+  <si>
+    <t>15\,123</t>
+  </si>
+  <si>
+    <t>4\,631</t>
+  </si>
+  <si>
+    <t>52\,190</t>
+  </si>
+  <si>
+    <t>60\,677</t>
+  </si>
+  <si>
+    <t>15\,050</t>
+  </si>
+  <si>
+    <t>1\,812</t>
+  </si>
+  <si>
+    <t>1\,789</t>
+  </si>
+  <si>
+    <t>14\,141</t>
+  </si>
+  <si>
+    <t>1\,922</t>
+  </si>
+  <si>
+    <t>6\,128</t>
   </si>
 </sst>
 </file>
@@ -4748,7 +4814,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A251" sqref="A251"/>
+      <selection pane="bottomLeft" activeCell="M136" sqref="M136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5644,7 +5710,7 @@
         <v>218</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>5</v>
@@ -10773,6 +10839,9 @@
       <c r="L131" s="11">
         <v>1</v>
       </c>
+      <c r="M131" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="N131" s="6" t="s">
         <v>159</v>
       </c>
@@ -10971,6 +11040,9 @@
       <c r="L135" s="11">
         <v>1</v>
       </c>
+      <c r="M135" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="N135" s="6" t="s">
         <v>159</v>
       </c>
@@ -13050,7 +13122,7 @@
         <v>745</v>
       </c>
       <c r="H190" s="9" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="I190" s="9" t="s">
         <v>1326</v>
@@ -15193,7 +15265,7 @@
         <v>748</v>
       </c>
       <c r="H251" s="9" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="I251" s="9" t="s">
         <v>1327</v>
@@ -19423,7 +19495,7 @@
         <v>761</v>
       </c>
       <c r="H371" s="9" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="I371" s="9" t="s">
         <v>1334</v>
@@ -24215,8 +24287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5C2734-B933-4C84-90BB-81AC6BC51564}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24226,35 +24298,38 @@
     <col min="4" max="4" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="C1" t="s">
         <v>1344</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C2" t="s">
         <v>1345</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="E2" t="s">
         <v>219</v>
@@ -24262,19 +24337,22 @@
       <c r="F2" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C3" t="s">
         <v>1346</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="E3" t="s">
         <v>243</v>
@@ -24282,19 +24360,22 @@
       <c r="F3" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C4" t="s">
         <v>1345</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="E4" t="s">
         <v>243</v>
@@ -24302,19 +24383,22 @@
       <c r="F4" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C5" t="s">
         <v>1346</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="E5" t="s">
         <v>219</v>
@@ -24322,53 +24406,62 @@
       <c r="F5" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C6" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C7" t="s">
         <v>1347</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="C8" t="s">
-        <v>1348</v>
+        <v>1405</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="E8" t="s">
         <v>219</v>
@@ -24376,19 +24469,22 @@
       <c r="F8" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="C9" t="s">
-        <v>1349</v>
+        <v>1406</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="E9" t="s">
         <v>243</v>
@@ -24396,19 +24492,22 @@
       <c r="F9" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="C10" t="s">
-        <v>1349</v>
+        <v>1406</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="E10" t="s">
         <v>219</v>
@@ -24416,19 +24515,22 @@
       <c r="F10" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="C11" t="s">
-        <v>1348</v>
+        <v>1405</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="E11" t="s">
         <v>243</v>
@@ -24436,19 +24538,22 @@
       <c r="F11" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C12" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="E12" t="s">
         <v>219</v>
@@ -24456,19 +24561,22 @@
       <c r="F12" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C13" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="E13" t="s">
         <v>243</v>
@@ -24476,19 +24584,22 @@
       <c r="F13" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C14" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="E14" t="s">
         <v>219</v>
@@ -24496,19 +24607,22 @@
       <c r="F14" s="9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C15" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="E15" t="s">
         <v>243</v>
@@ -24516,22 +24630,28 @@
       <c r="F15" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="C16" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1414</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -24539,16 +24659,19 @@
         <v>48</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="C17" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>243</v>
+      </c>
+      <c r="G17">
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -24556,16 +24679,19 @@
         <v>60</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C18" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1417</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -24573,16 +24699,19 @@
         <v>60</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C19" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>243</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1418</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -24590,19 +24719,22 @@
         <v>120</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="C20" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="E20" t="s">
         <v>219</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1419</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -24610,19 +24742,22 @@
         <v>124</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C21" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="E21" t="s">
         <v>219</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1420</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -24630,19 +24765,22 @@
         <v>154</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C22" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="E22" t="s">
         <v>219</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1422</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -24650,19 +24788,22 @@
         <v>154</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C23" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="E23" t="s">
         <v>243</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>243</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1421</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -24670,19 +24811,22 @@
         <v>154</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C24" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="E24" t="s">
         <v>219</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>243</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1421</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -24690,19 +24834,22 @@
         <v>154</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C25" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="E25" t="s">
         <v>243</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1422</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -24710,16 +24857,19 @@
         <v>170</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="C26" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1423</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -24727,16 +24877,19 @@
         <v>118</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C27" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>219</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1425</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -24744,16 +24897,19 @@
         <v>118</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C28" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>243</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1424</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -24761,19 +24917,21 @@
         <v>50</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="C29" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" t="s">
+        <v>1415</v>
+      </c>
       <c r="H29" s="6"/>
       <c r="I29" s="9"/>
       <c r="J29" s="6"/>
@@ -24783,19 +24941,21 @@
         <v>50</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="C30" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="G30" s="6"/>
+      <c r="G30" t="s">
+        <v>1416</v>
+      </c>
       <c r="H30" s="6"/>
       <c r="I30" s="9"/>
       <c r="J30" s="6"/>
@@ -24805,19 +24965,21 @@
         <v>72</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="C31" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="G31" s="6"/>
+      <c r="G31" t="s">
+        <v>1426</v>
+      </c>
       <c r="H31" s="6"/>
       <c r="I31" s="9"/>
       <c r="J31" s="6"/>
@@ -24827,19 +24989,21 @@
         <v>184</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="C32" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="G32" s="6"/>
+      <c r="G32" t="s">
+        <v>1428</v>
+      </c>
       <c r="H32" s="6"/>
       <c r="I32" s="9"/>
       <c r="J32" s="6"/>
@@ -24849,19 +25013,21 @@
         <v>184</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C33" t="s">
         <v>1399</v>
       </c>
-      <c r="C33" t="s">
-        <v>1401</v>
-      </c>
       <c r="D33" s="9" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="G33" s="6"/>
+      <c r="G33" t="s">
+        <v>1427</v>
+      </c>
       <c r="H33" s="6"/>
       <c r="I33" s="9"/>
       <c r="J33" s="6"/>

</xml_diff>

<commit_message>
work on lingu background
</commit_message>
<xml_diff>
--- a/data/phoneticData.xlsx
+++ b/data/phoneticData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9631F66-CED1-4C7F-AF92-65FDEDBCBAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC0FBA8-CD43-42E5-A25B-221E1E3D2083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5970" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5994" uniqueCount="1430">
   <si>
     <t>iso639_3</t>
   </si>
@@ -4332,6 +4332,9 @@
   </si>
   <si>
     <t>6\,128</t>
+  </si>
+  <si>
+    <t>unk</t>
   </si>
 </sst>
 </file>
@@ -4812,9 +4815,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Z509"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M136" sqref="M136"/>
+      <selection pane="bottomLeft" activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4954,6 +4957,9 @@
       <c r="C3" s="9" t="s">
         <v>325</v>
       </c>
+      <c r="D3" s="9" t="s">
+        <v>1429</v>
+      </c>
       <c r="E3" s="10">
         <v>20</v>
       </c>
@@ -4998,6 +5004,9 @@
       <c r="C4" s="9" t="s">
         <v>331</v>
       </c>
+      <c r="D4" s="9" t="s">
+        <v>1429</v>
+      </c>
       <c r="E4" s="10">
         <v>300000</v>
       </c>
@@ -5235,6 +5244,9 @@
       <c r="C9" s="9" t="s">
         <v>325</v>
       </c>
+      <c r="D9" s="9" t="s">
+        <v>1429</v>
+      </c>
       <c r="F9" s="9" t="s">
         <v>218</v>
       </c>
@@ -5705,6 +5717,9 @@
       </c>
       <c r="C19" s="9" t="s">
         <v>325</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>218</v>
@@ -6173,6 +6188,9 @@
       <c r="D30" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E30" s="10">
+        <v>79</v>
+      </c>
       <c r="F30" s="9" t="s">
         <v>218</v>
       </c>
@@ -6222,6 +6240,9 @@
       <c r="D31" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E31" s="10">
+        <v>79</v>
+      </c>
       <c r="F31" s="9" t="s">
         <v>218</v>
       </c>
@@ -6307,7 +6328,7 @@
       <c r="W32" s="2"/>
       <c r="Y32" s="3"/>
     </row>
-    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>36</v>
       </c>
@@ -6316,6 +6337,9 @@
       </c>
       <c r="C33" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>218</v>
@@ -7831,7 +7855,7 @@
       <c r="W68" s="2"/>
       <c r="Y68" s="3"/>
     </row>
-    <row r="69" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>96</v>
       </c>
@@ -7840,6 +7864,9 @@
       </c>
       <c r="C69" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>218</v>
@@ -7932,6 +7959,12 @@
       </c>
       <c r="C71" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E71" s="10">
+        <v>552</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>218</v>
@@ -8982,7 +9015,7 @@
       <c r="W91" s="2"/>
       <c r="Y91" s="3"/>
     </row>
-    <row r="92" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>160</v>
       </c>
@@ -9028,7 +9061,7 @@
       <c r="W92" s="2"/>
       <c r="Y92" s="3"/>
     </row>
-    <row r="93" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>160</v>
       </c>
@@ -9087,6 +9120,9 @@
       <c r="D94" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E94" s="10">
+        <v>108</v>
+      </c>
       <c r="F94" s="9" t="s">
         <v>218</v>
       </c>
@@ -9136,6 +9172,9 @@
       </c>
       <c r="D95" s="9" t="s">
         <v>243</v>
+      </c>
+      <c r="E95" s="10">
+        <v>108</v>
       </c>
       <c r="F95" s="9" t="s">
         <v>218</v>
@@ -9738,7 +9777,7 @@
       <c r="X108" s="1"/>
       <c r="Y108" s="3"/>
     </row>
-    <row r="109" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>112</v>
       </c>
@@ -9795,6 +9834,12 @@
       <c r="C110" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D110" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E110" s="10">
+        <v>114</v>
+      </c>
       <c r="F110" s="9" t="s">
         <v>218</v>
       </c>
@@ -10042,6 +10087,9 @@
       <c r="C115" s="9" t="s">
         <v>291</v>
       </c>
+      <c r="D115" s="9" t="s">
+        <v>1429</v>
+      </c>
       <c r="E115" s="10">
         <v>217664</v>
       </c>
@@ -10079,7 +10127,7 @@
       <c r="X115" s="1"/>
       <c r="Y115" s="3"/>
     </row>
-    <row r="116" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>158</v>
       </c>
@@ -10126,7 +10174,7 @@
       <c r="X116" s="1"/>
       <c r="Y116" s="3"/>
     </row>
-    <row r="117" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>158</v>
       </c>
@@ -10173,7 +10221,7 @@
       <c r="X117" s="1"/>
       <c r="Y117" s="3"/>
     </row>
-    <row r="118" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>158</v>
       </c>
@@ -10220,7 +10268,7 @@
       <c r="X118" s="1"/>
       <c r="Y118" s="3"/>
     </row>
-    <row r="119" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>158</v>
       </c>
@@ -10267,7 +10315,7 @@
       <c r="X119" s="1"/>
       <c r="Y119" s="3"/>
     </row>
-    <row r="120" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>158</v>
       </c>
@@ -10324,6 +10372,9 @@
       <c r="C121" s="9" t="s">
         <v>291</v>
       </c>
+      <c r="D121" s="9" t="s">
+        <v>1429</v>
+      </c>
       <c r="E121" s="10">
         <v>41000</v>
       </c>
@@ -10713,7 +10764,7 @@
       <c r="X128" s="1"/>
       <c r="Y128" s="3"/>
     </row>
-    <row r="129" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>158</v>
       </c>
@@ -10760,7 +10811,7 @@
       <c r="X129" s="1"/>
       <c r="Y129" s="3"/>
     </row>
-    <row r="130" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>158</v>
       </c>
@@ -10820,6 +10871,9 @@
       <c r="D131" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E131" s="10">
+        <v>113</v>
+      </c>
       <c r="F131" s="9" t="s">
         <v>218</v>
       </c>
@@ -11021,6 +11075,9 @@
       <c r="D135" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E135" s="10">
+        <v>113</v>
+      </c>
       <c r="F135" s="9" t="s">
         <v>218</v>
       </c>
@@ -11072,6 +11129,9 @@
       <c r="D136" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E136" s="10">
+        <v>99</v>
+      </c>
       <c r="F136" s="9" t="s">
         <v>218</v>
       </c>
@@ -11125,6 +11185,9 @@
       <c r="D137" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E137" s="10">
+        <v>99</v>
+      </c>
       <c r="F137" s="9" t="s">
         <v>218</v>
       </c>
@@ -11613,7 +11676,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>156</v>
       </c>
@@ -12958,6 +13021,9 @@
       <c r="D186" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E186" s="10">
+        <v>169</v>
+      </c>
       <c r="F186" s="9" t="s">
         <v>218</v>
       </c>
@@ -13074,6 +13140,12 @@
       <c r="C189" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D189" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E189" s="10">
+        <v>90</v>
+      </c>
       <c r="F189" s="9" t="s">
         <v>218</v>
       </c>
@@ -13115,6 +13187,9 @@
       <c r="D190" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E190" s="10">
+        <v>129</v>
+      </c>
       <c r="F190" s="9" t="s">
         <v>218</v>
       </c>
@@ -13744,6 +13819,12 @@
       <c r="C208" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D208" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E208" s="10">
+        <v>139</v>
+      </c>
       <c r="F208" s="9" t="s">
         <v>218</v>
       </c>
@@ -14220,7 +14301,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="221" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
         <v>126</v>
       </c>
@@ -14229,6 +14310,9 @@
       </c>
       <c r="C221" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D221" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F221" s="9" t="s">
         <v>218</v>
@@ -14559,6 +14643,9 @@
       <c r="D230" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E230" s="10">
+        <v>107</v>
+      </c>
       <c r="F230" s="9" t="s">
         <v>218</v>
       </c>
@@ -14600,6 +14687,9 @@
       <c r="D231" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E231" s="10">
+        <v>107</v>
+      </c>
       <c r="F231" s="9" t="s">
         <v>218</v>
       </c>
@@ -15213,7 +15303,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="250" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
         <v>72</v>
       </c>
@@ -15222,6 +15312,9 @@
       </c>
       <c r="C250" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D250" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F250" s="9" t="s">
         <v>218</v>
@@ -15258,6 +15351,12 @@
       <c r="C251" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D251" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E251" s="10">
+        <v>64</v>
+      </c>
       <c r="F251" s="9" t="s">
         <v>218</v>
       </c>
@@ -15296,6 +15395,9 @@
       <c r="C252" s="9" t="s">
         <v>291</v>
       </c>
+      <c r="D252" s="9" t="s">
+        <v>1429</v>
+      </c>
       <c r="E252" s="10">
         <v>10000</v>
       </c>
@@ -17568,7 +17670,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="318" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
         <v>124</v>
       </c>
@@ -17577,6 +17679,9 @@
       </c>
       <c r="C318" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D318" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F318" s="9" t="s">
         <v>218</v>
@@ -17610,6 +17715,12 @@
       <c r="C319" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D319" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E319" s="10">
+        <v>42</v>
+      </c>
       <c r="F319" s="9" t="s">
         <v>218</v>
       </c>
@@ -19328,7 +19439,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="367" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A367" s="6" t="s">
         <v>184</v>
       </c>
@@ -19337,6 +19448,9 @@
       </c>
       <c r="C367" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D367" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F367" s="9" t="s">
         <v>218</v>
@@ -19488,6 +19602,12 @@
       <c r="C371" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D371" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E371" s="10">
+        <v>91</v>
+      </c>
       <c r="F371" s="9" t="s">
         <v>218</v>
       </c>
@@ -20330,7 +20450,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="397" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A397" s="6" t="s">
         <v>146</v>
       </c>
@@ -21269,7 +21389,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="423" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A423" s="6" t="s">
         <v>154</v>
       </c>
@@ -21320,6 +21440,9 @@
       <c r="D424" s="9" t="s">
         <v>243</v>
       </c>
+      <c r="E424" s="10">
+        <v>97</v>
+      </c>
       <c r="F424" s="9" t="s">
         <v>218</v>
       </c>
@@ -21364,6 +21487,9 @@
       <c r="D425" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E425" s="10">
+        <v>97</v>
+      </c>
       <c r="F425" s="9" t="s">
         <v>218</v>
       </c>
@@ -22298,7 +22424,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="449" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A449" s="6" t="s">
         <v>164</v>
       </c>
@@ -22307,6 +22433,9 @@
       </c>
       <c r="C449" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D449" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F449" s="9" t="s">
         <v>218</v>
@@ -22413,7 +22542,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="452" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A452" s="6" t="s">
         <v>170</v>
       </c>
@@ -22422,6 +22551,9 @@
       </c>
       <c r="C452" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D452" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F452" s="9" t="s">
         <v>218</v>
@@ -22458,6 +22590,12 @@
       <c r="C453" s="9" t="s">
         <v>226</v>
       </c>
+      <c r="D453" s="9" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E453" s="10">
+        <v>21</v>
+      </c>
       <c r="F453" s="9" t="s">
         <v>218</v>
       </c>
@@ -22810,7 +22948,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="464" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A464" s="6" t="s">
         <v>118</v>
       </c>
@@ -22861,6 +22999,9 @@
       <c r="D465" s="9" t="s">
         <v>219</v>
       </c>
+      <c r="E465" s="10">
+        <v>65</v>
+      </c>
       <c r="F465" s="9" t="s">
         <v>218</v>
       </c>
@@ -24061,7 +24202,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="505" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A505" s="6" t="s">
         <v>198</v>
       </c>
@@ -24070,6 +24211,9 @@
       </c>
       <c r="C505" s="9" t="s">
         <v>226</v>
+      </c>
+      <c r="D505" s="9" t="s">
+        <v>1429</v>
       </c>
       <c r="F505" s="9" t="s">
         <v>218</v>
@@ -24252,11 +24396,6 @@
       <filters>
         <filter val="full text (the north wind and the sun)"/>
       </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
     </filterColumn>
     <filterColumn colId="14">
       <filters>
@@ -24287,7 +24426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5C2734-B933-4C84-90BB-81AC6BC51564}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
word len means done
</commit_message>
<xml_diff>
--- a/data/phoneticData.xlsx
+++ b/data/phoneticData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debor\masterThesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A9FB2-8070-4B27-9D2A-71052F58363C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318362F2-1ECC-4393-A008-B8146948961D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4132,15 +4132,6 @@
     <t>alamblak.pdf</t>
   </si>
   <si>
-    <t>theNorthWindAndTheSun\pes-orthographic.txt</t>
-  </si>
-  <si>
-    <t>theNorthWindAndTheSun\kor-orthographic.txt</t>
-  </si>
-  <si>
-    <t>theNorthWindAndTheSun\hin-orthographic.txt</t>
-  </si>
-  <si>
     <t>C:/Users/debor/masterThesis/data/theNorthWindAndTheSun/cmn.txt</t>
   </si>
   <si>
@@ -4390,12 +4381,6 @@
     <t>Nahuatl</t>
   </si>
   <si>
-    <t>theNorthWindandTheSun/fra.txt</t>
-  </si>
-  <si>
-    <t>theNorthWindandTheSun/fra-orthographic.txt</t>
-  </si>
-  <si>
     <t>theNorthWindAndTheSun/eus-goizueta-broad.txt</t>
   </si>
   <si>
@@ -4463,6 +4448,21 @@
   </si>
   <si>
     <t>theNorthWindAndTheSun/kat-orthographic.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun/fra.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun/fra-orthographic.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun/hin-orthographic.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun/kor-orthographic.txt</t>
+  </si>
+  <si>
+    <t>theNorthWindAndTheSun/pes-orthographic.txt</t>
   </si>
 </sst>
 </file>
@@ -4974,8 +4974,8 @@
   <dimension ref="A1:AA522"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D220" sqref="D220"/>
+      <pane ySplit="1" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I481" sqref="I481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5017,7 +5017,7 @@
         <v>290</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>217</v>
@@ -5053,10 +5053,10 @@
         <v>719</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
@@ -5125,13 +5125,13 @@
         <v>325</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E3" s="10">
         <v>20</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="H3" s="8"/>
       <c r="K3" s="9" t="s">
@@ -5169,13 +5169,13 @@
         <v>331</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E4" s="10">
         <v>300000</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>326</v>
@@ -5412,25 +5412,25 @@
         <v>325</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E9" s="10">
         <v>109</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>218</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>1468</v>
+        <v>1463</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>328</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>293</v>
@@ -5864,7 +5864,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>323</v>
@@ -5873,7 +5873,7 @@
         <v>334</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
@@ -5894,7 +5894,7 @@
         <v>325</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>218</v>
@@ -6367,7 +6367,7 @@
         <v>79</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>218</v>
@@ -6422,7 +6422,7 @@
         <v>79</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>218</v>
@@ -6477,7 +6477,7 @@
         <v>113</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>218</v>
@@ -6504,7 +6504,7 @@
         <v>338</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
@@ -6525,7 +6525,7 @@
         <v>226</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>218</v>
@@ -7333,7 +7333,7 @@
     </row>
     <row r="51" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>293</v>
@@ -7360,16 +7360,16 @@
         <v>0</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="P51" s="9" t="s">
         <v>323</v>
       </c>
       <c r="Q51" s="6" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
@@ -8051,7 +8051,7 @@
         <v>226</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G69" s="9" t="s">
         <v>218</v>
@@ -8103,7 +8103,7 @@
         <v>133686</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G70" s="6" t="s">
         <v>218</v>
@@ -8130,7 +8130,7 @@
         <v>396</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
@@ -8151,13 +8151,13 @@
         <v>226</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E71" s="10">
         <v>552</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G71" s="9" t="s">
         <v>218</v>
@@ -8461,7 +8461,7 @@
         <v>152</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>218</v>
@@ -8488,7 +8488,7 @@
         <v>405</v>
       </c>
       <c r="R77" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
@@ -8515,7 +8515,7 @@
         <v>193</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>218</v>
@@ -8542,7 +8542,7 @@
         <v>334</v>
       </c>
       <c r="R78" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
@@ -9038,7 +9038,7 @@
         <v>35486</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>218</v>
@@ -9063,7 +9063,7 @@
         <v>334</v>
       </c>
       <c r="R88" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
@@ -9090,7 +9090,7 @@
         <v>34145</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>218</v>
@@ -9115,7 +9115,7 @@
         <v>334</v>
       </c>
       <c r="R89" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
@@ -9142,7 +9142,7 @@
         <v>10984</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>218</v>
@@ -9167,7 +9167,7 @@
         <v>334</v>
       </c>
       <c r="R90" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
@@ -9180,7 +9180,7 @@
     </row>
     <row r="91" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>293</v>
@@ -9207,16 +9207,16 @@
         <v>0</v>
       </c>
       <c r="O91" s="6" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="P91" s="9" t="s">
         <v>323</v>
       </c>
       <c r="Q91" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="R91" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
@@ -9335,7 +9335,7 @@
         <v>108</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G94" s="9" t="s">
         <v>218</v>
@@ -9391,7 +9391,7 @@
         <v>108</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G95" s="9" t="s">
         <v>218</v>
@@ -9917,7 +9917,7 @@
         <v>10626</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>218</v>
@@ -9944,7 +9944,7 @@
         <v>455</v>
       </c>
       <c r="R107" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
@@ -9972,7 +9972,7 @@
         <v>10547</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G108" s="6" t="s">
         <v>218</v>
@@ -9999,7 +9999,7 @@
         <v>455</v>
       </c>
       <c r="R108" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
@@ -10071,13 +10071,13 @@
         <v>226</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E110" s="10">
         <v>114</v>
       </c>
       <c r="F110" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G110" s="9" t="s">
         <v>218</v>
@@ -10110,10 +10110,10 @@
         <v>455</v>
       </c>
       <c r="R110" s="15" t="s">
+        <v>1447</v>
+      </c>
+      <c r="S110" s="15" t="s">
         <v>1452</v>
-      </c>
-      <c r="S110" s="15" t="s">
-        <v>1457</v>
       </c>
       <c r="T110" s="2"/>
       <c r="U110" s="2"/>
@@ -10140,7 +10140,7 @@
         <v>408</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>218</v>
@@ -10167,7 +10167,7 @@
         <v>455</v>
       </c>
       <c r="R111" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
@@ -10189,13 +10189,13 @@
         <v>291</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E112" s="10">
         <v>217664</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G112" s="9" t="s">
         <v>218</v>
@@ -10242,13 +10242,13 @@
         <v>291</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E113" s="10">
         <v>41000</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G113" s="9" t="s">
         <v>218</v>
@@ -10273,7 +10273,7 @@
         <v>324</v>
       </c>
       <c r="R113" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
@@ -10301,7 +10301,7 @@
         <v>61173</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>218</v>
@@ -10329,7 +10329,7 @@
         <v>334</v>
       </c>
       <c r="R114" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
@@ -10357,7 +10357,7 @@
         <v>60422</v>
       </c>
       <c r="F115" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>218</v>
@@ -10385,7 +10385,7 @@
         <v>334</v>
       </c>
       <c r="R115" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
@@ -10663,7 +10663,7 @@
         <v>1284</v>
       </c>
       <c r="F121" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G121" s="6" t="s">
         <v>218</v>
@@ -10691,7 +10691,7 @@
         <v>334</v>
       </c>
       <c r="R121" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S121" s="2"/>
       <c r="T121" s="2"/>
@@ -10719,7 +10719,7 @@
         <v>58072</v>
       </c>
       <c r="F122" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>218</v>
@@ -10747,7 +10747,7 @@
         <v>334</v>
       </c>
       <c r="R122" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
@@ -10775,7 +10775,7 @@
         <v>57230</v>
       </c>
       <c r="F123" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>218</v>
@@ -10803,7 +10803,7 @@
         <v>334</v>
       </c>
       <c r="R123" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S123" s="2"/>
       <c r="T123" s="2"/>
@@ -10831,7 +10831,7 @@
         <v>1633</v>
       </c>
       <c r="F124" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>218</v>
@@ -10859,7 +10859,7 @@
         <v>334</v>
       </c>
       <c r="R124" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S124" s="2"/>
       <c r="T124" s="2"/>
@@ -10972,7 +10972,7 @@
     </row>
     <row r="127" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="6" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="B127" s="9" t="s">
         <v>293</v>
@@ -10999,16 +10999,16 @@
         <v>0</v>
       </c>
       <c r="O127" s="6" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
       <c r="P127" s="9" t="s">
         <v>323</v>
       </c>
       <c r="Q127" s="6" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
       <c r="R127" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S127" s="2"/>
       <c r="T127" s="2"/>
@@ -11136,17 +11136,17 @@
         <v>113</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G130" s="9" t="s">
         <v>218</v>
       </c>
       <c r="H130" s="8"/>
       <c r="I130" s="9" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="J130" s="9" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="K130" s="9" t="s">
         <v>765</v>
@@ -11196,17 +11196,17 @@
         <v>113</v>
       </c>
       <c r="F131" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G131" s="9" t="s">
         <v>218</v>
       </c>
       <c r="H131" s="8"/>
       <c r="I131" s="9" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="J131" s="9" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="K131" s="9" t="s">
         <v>765</v>
@@ -11256,7 +11256,7 @@
         <v>1742</v>
       </c>
       <c r="F132" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G132" s="6" t="s">
         <v>218</v>
@@ -11281,7 +11281,7 @@
         <v>334</v>
       </c>
       <c r="R132" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S132" s="2"/>
       <c r="T132" s="2"/>
@@ -11409,7 +11409,7 @@
         <v>186</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>218</v>
@@ -11434,7 +11434,7 @@
         <v>334</v>
       </c>
       <c r="R135" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S135" s="2"/>
       <c r="T135" s="2"/>
@@ -11462,7 +11462,7 @@
         <v>99</v>
       </c>
       <c r="F136" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G136" s="9" t="s">
         <v>218</v>
@@ -11471,10 +11471,10 @@
         <v>732</v>
       </c>
       <c r="I136" s="6" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
       <c r="J136" s="6" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
       <c r="K136" s="9" t="s">
         <v>733</v>
@@ -11495,7 +11495,7 @@
         <v>324</v>
       </c>
       <c r="R136" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="S136" s="15"/>
       <c r="T136" s="2"/>
@@ -11523,7 +11523,7 @@
         <v>99</v>
       </c>
       <c r="F137" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G137" s="9" t="s">
         <v>218</v>
@@ -11532,10 +11532,10 @@
         <v>732</v>
       </c>
       <c r="I137" s="6" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
       <c r="J137" s="6" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
       <c r="K137" s="9" t="s">
         <v>733</v>
@@ -11556,7 +11556,7 @@
         <v>324</v>
       </c>
       <c r="R137" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="S137" s="15"/>
       <c r="T137" s="2"/>
@@ -11752,7 +11752,7 @@
         <v>69015</v>
       </c>
       <c r="F142" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G142" s="6" t="s">
         <v>218</v>
@@ -11778,7 +11778,7 @@
         <v>334</v>
       </c>
       <c r="R142" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S142" s="2"/>
     </row>
@@ -11799,7 +11799,7 @@
         <v>69008</v>
       </c>
       <c r="F143" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G143" s="6" t="s">
         <v>218</v>
@@ -11825,7 +11825,7 @@
         <v>334</v>
       </c>
       <c r="R143" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S143"/>
     </row>
@@ -11846,7 +11846,7 @@
         <v>57029</v>
       </c>
       <c r="F144" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G144" s="6" t="s">
         <v>218</v>
@@ -11872,7 +11872,7 @@
         <v>334</v>
       </c>
       <c r="R144" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S144"/>
     </row>
@@ -11893,7 +11893,7 @@
         <v>56911</v>
       </c>
       <c r="F145" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G145" s="6" t="s">
         <v>218</v>
@@ -11919,7 +11919,7 @@
         <v>334</v>
       </c>
       <c r="R145" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S145"/>
     </row>
@@ -11940,7 +11940,7 @@
         <v>194</v>
       </c>
       <c r="F146" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G146" s="6" t="s">
         <v>218</v>
@@ -11966,7 +11966,7 @@
         <v>334</v>
       </c>
       <c r="R146" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S146"/>
     </row>
@@ -12076,10 +12076,10 @@
         <v>206</v>
       </c>
       <c r="I149" s="9" t="s">
-        <v>1448</v>
+        <v>1468</v>
       </c>
       <c r="J149" s="9" t="s">
-        <v>1447</v>
+        <v>1467</v>
       </c>
       <c r="K149" s="9" t="s">
         <v>208</v>
@@ -12100,7 +12100,7 @@
         <v>324</v>
       </c>
       <c r="R149" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="150" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
@@ -12739,7 +12739,7 @@
     </row>
     <row r="165" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="B165" s="9" t="s">
         <v>293</v>
@@ -12766,16 +12766,16 @@
         <v>0</v>
       </c>
       <c r="O165" s="6" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
       <c r="P165" s="9" t="s">
         <v>323</v>
       </c>
       <c r="Q165" s="6" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
       <c r="R165" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S165"/>
     </row>
@@ -13232,7 +13232,7 @@
         <v>169</v>
       </c>
       <c r="F180" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G180" s="9" t="s">
         <v>218</v>
@@ -13275,13 +13275,13 @@
         <v>226</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E181" s="10">
         <v>90</v>
       </c>
       <c r="F181" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G181" s="9" t="s">
         <v>218</v>
@@ -13330,7 +13330,7 @@
         <v>11296</v>
       </c>
       <c r="F182" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G182" s="6" t="s">
         <v>218</v>
@@ -13356,7 +13356,7 @@
         <v>460</v>
       </c>
       <c r="R182" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S182"/>
     </row>
@@ -13503,7 +13503,7 @@
         <v>10812</v>
       </c>
       <c r="F186" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G186" s="6" t="s">
         <v>218</v>
@@ -13529,7 +13529,7 @@
         <v>460</v>
       </c>
       <c r="R186" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S186"/>
     </row>
@@ -13634,7 +13634,7 @@
         <v>9563</v>
       </c>
       <c r="F189" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G189" s="6" t="s">
         <v>218</v>
@@ -13660,7 +13660,7 @@
         <v>460</v>
       </c>
       <c r="R189" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S189"/>
     </row>
@@ -13681,7 +13681,7 @@
         <v>129</v>
       </c>
       <c r="F190" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G190" s="9" t="s">
         <v>218</v>
@@ -13690,7 +13690,7 @@
         <v>745</v>
       </c>
       <c r="I190" s="9" t="s">
-        <v>1363</v>
+        <v>1469</v>
       </c>
       <c r="J190" s="9" t="s">
         <v>1317</v>
@@ -13711,7 +13711,7 @@
         <v>324</v>
       </c>
       <c r="R190" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="191" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
@@ -14234,7 +14234,7 @@
         <v>1555</v>
       </c>
       <c r="F205" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G205" s="6" t="s">
         <v>218</v>
@@ -14260,7 +14260,7 @@
         <v>334</v>
       </c>
       <c r="R205" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S205"/>
     </row>
@@ -14323,7 +14323,7 @@
         <v>2637</v>
       </c>
       <c r="F207" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G207" s="6" t="s">
         <v>218</v>
@@ -14349,7 +14349,7 @@
         <v>334</v>
       </c>
       <c r="R207" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S207"/>
     </row>
@@ -14364,13 +14364,13 @@
         <v>226</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E208" s="10">
         <v>139</v>
       </c>
       <c r="F208" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G208" s="9" t="s">
         <v>218</v>
@@ -14681,7 +14681,7 @@
         <v>19930</v>
       </c>
       <c r="F216" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G216" s="6" t="s">
         <v>218</v>
@@ -14707,7 +14707,7 @@
         <v>480</v>
       </c>
       <c r="R216" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S216"/>
     </row>
@@ -14728,7 +14728,7 @@
         <v>19689</v>
       </c>
       <c r="F217" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G217" s="6" t="s">
         <v>218</v>
@@ -14754,7 +14754,7 @@
         <v>480</v>
       </c>
       <c r="R217" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S217"/>
     </row>
@@ -14775,7 +14775,7 @@
         <v>5268</v>
       </c>
       <c r="F218" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>218</v>
@@ -14801,7 +14801,7 @@
         <v>481</v>
       </c>
       <c r="R218" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S218"/>
     </row>
@@ -14822,7 +14822,7 @@
         <v>4765</v>
       </c>
       <c r="F219" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G219" s="6" t="s">
         <v>218</v>
@@ -14848,7 +14848,7 @@
         <v>481</v>
       </c>
       <c r="R219" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S219"/>
     </row>
@@ -14863,7 +14863,7 @@
         <v>226</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G220" s="9" t="s">
         <v>218</v>
@@ -14872,10 +14872,10 @@
         <v>206</v>
       </c>
       <c r="I220" s="9" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="J220" s="9" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="K220" s="13" t="s">
         <v>208</v>
@@ -14896,7 +14896,7 @@
         <v>324</v>
       </c>
       <c r="R220" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="221" spans="1:19" x14ac:dyDescent="0.35">
@@ -14916,7 +14916,7 @@
         <v>173</v>
       </c>
       <c r="F221" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G221" s="6" t="s">
         <v>218</v>
@@ -14942,7 +14942,7 @@
         <v>334</v>
       </c>
       <c r="R221" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S221"/>
     </row>
@@ -14963,7 +14963,7 @@
         <v>100</v>
       </c>
       <c r="F222" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G222" s="9" t="s">
         <v>218</v>
@@ -14987,7 +14987,7 @@
         <v>123</v>
       </c>
       <c r="R222" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S222"/>
     </row>
@@ -15092,7 +15092,7 @@
         <v>15124</v>
       </c>
       <c r="F225" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G225" s="6" t="s">
         <v>218</v>
@@ -15118,7 +15118,7 @@
         <v>121</v>
       </c>
       <c r="R225" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S225"/>
     </row>
@@ -15139,7 +15139,7 @@
         <v>15123</v>
       </c>
       <c r="F226" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G226" s="6" t="s">
         <v>218</v>
@@ -15165,7 +15165,7 @@
         <v>121</v>
       </c>
       <c r="R226" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S226"/>
     </row>
@@ -15270,7 +15270,7 @@
         <v>107</v>
       </c>
       <c r="F229" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G229" s="9" t="s">
         <v>218</v>
@@ -15279,7 +15279,7 @@
         <v>737</v>
       </c>
       <c r="I229" s="9" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="J229" s="9" t="s">
         <v>1320</v>
@@ -15319,7 +15319,7 @@
         <v>107</v>
       </c>
       <c r="F230" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G230" s="9" t="s">
         <v>218</v>
@@ -15328,7 +15328,7 @@
         <v>737</v>
       </c>
       <c r="I230" s="9" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="J230" s="9" t="s">
         <v>1321</v>
@@ -15763,13 +15763,13 @@
         <v>291</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E244" s="10">
         <v>10000</v>
       </c>
       <c r="F244" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G244" s="9" t="s">
         <v>218</v>
@@ -15790,7 +15790,7 @@
         <v>324</v>
       </c>
       <c r="R244" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S244"/>
     </row>
@@ -15811,7 +15811,7 @@
         <v>16402</v>
       </c>
       <c r="F245" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G245" s="6" t="s">
         <v>218</v>
@@ -15837,7 +15837,7 @@
         <v>479</v>
       </c>
       <c r="R245" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S245"/>
     </row>
@@ -15885,7 +15885,7 @@
     </row>
     <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" s="6" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="B247" s="9" t="s">
         <v>293</v>
@@ -15912,7 +15912,7 @@
         <v>0</v>
       </c>
       <c r="O247" s="6" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
       <c r="P247" s="9" t="s">
         <v>323</v>
@@ -15921,7 +15921,7 @@
         <v>334</v>
       </c>
       <c r="R247" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S247"/>
     </row>
@@ -15942,7 +15942,7 @@
         <v>14141</v>
       </c>
       <c r="F248" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G248" s="6" t="s">
         <v>218</v>
@@ -15968,7 +15968,7 @@
         <v>479</v>
       </c>
       <c r="R248" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S248"/>
     </row>
@@ -15983,7 +15983,7 @@
         <v>226</v>
       </c>
       <c r="D249" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G249" s="9" t="s">
         <v>218</v>
@@ -16023,13 +16023,13 @@
         <v>226</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E250" s="10">
         <v>64</v>
       </c>
       <c r="F250" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G250" s="9" t="s">
         <v>218</v>
@@ -16038,7 +16038,7 @@
         <v>748</v>
       </c>
       <c r="I250" s="9" t="s">
-        <v>1362</v>
+        <v>1470</v>
       </c>
       <c r="J250" s="9" t="s">
         <v>1318</v>
@@ -18339,7 +18339,7 @@
         <v>4636</v>
       </c>
       <c r="F313" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G313" s="6" t="s">
         <v>218</v>
@@ -18365,7 +18365,7 @@
         <v>385</v>
       </c>
       <c r="R313" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S313"/>
     </row>
@@ -18473,7 +18473,7 @@
         <v>4631</v>
       </c>
       <c r="F316" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G316" s="6" t="s">
         <v>218</v>
@@ -18499,7 +18499,7 @@
         <v>385</v>
       </c>
       <c r="R316" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S316"/>
     </row>
@@ -18514,7 +18514,7 @@
         <v>226</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G317" s="9" t="s">
         <v>218</v>
@@ -18551,13 +18551,13 @@
         <v>226</v>
       </c>
       <c r="D318" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E318" s="10">
         <v>42</v>
       </c>
       <c r="F318" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G318" s="9" t="s">
         <v>218</v>
@@ -18587,7 +18587,7 @@
         <v>324</v>
       </c>
       <c r="R318" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="319" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
@@ -19004,7 +19004,7 @@
     </row>
     <row r="331" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A331" s="6" t="s">
-        <v>1433</v>
+        <v>1430</v>
       </c>
       <c r="B331" s="9" t="s">
         <v>293</v>
@@ -19031,10 +19031,10 @@
         <v>0</v>
       </c>
       <c r="N331" s="6" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
       <c r="O331" s="6" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="P331" s="9" t="s">
         <v>323</v>
@@ -19043,7 +19043,7 @@
         <v>334</v>
       </c>
       <c r="R331" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S331"/>
     </row>
@@ -20370,7 +20370,7 @@
         <v>226</v>
       </c>
       <c r="D366" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G366" s="9" t="s">
         <v>218</v>
@@ -20537,13 +20537,13 @@
         <v>226</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E370" s="10">
         <v>91</v>
       </c>
       <c r="F370" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G370" s="9" t="s">
         <v>218</v>
@@ -20552,7 +20552,7 @@
         <v>761</v>
       </c>
       <c r="I370" s="9" t="s">
-        <v>1361</v>
+        <v>1471</v>
       </c>
       <c r="J370" s="9" t="s">
         <v>1324</v>
@@ -20883,7 +20883,7 @@
     </row>
     <row r="378" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A378" s="6" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
       <c r="B378" s="9" t="s">
         <v>293</v>
@@ -20910,7 +20910,7 @@
         <v>0</v>
       </c>
       <c r="O378" s="6" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
       <c r="P378" s="9" t="s">
         <v>323</v>
@@ -20919,7 +20919,7 @@
         <v>334</v>
       </c>
       <c r="R378" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S378"/>
     </row>
@@ -21163,20 +21163,20 @@
         <v>226</v>
       </c>
       <c r="D386" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E386" s="10">
         <v>87</v>
       </c>
       <c r="F386" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G386" s="9" t="s">
         <v>218</v>
       </c>
       <c r="H386" s="8"/>
       <c r="J386" s="9" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="L386" s="12">
         <v>44490</v>
@@ -21191,7 +21191,7 @@
         <v>324</v>
       </c>
       <c r="R386" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="S386"/>
     </row>
@@ -21254,7 +21254,7 @@
         <v>402586</v>
       </c>
       <c r="F390" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G390" s="6" t="s">
         <v>218</v>
@@ -21279,7 +21279,7 @@
         <v>341</v>
       </c>
       <c r="R390" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S390"/>
     </row>
@@ -21462,20 +21462,20 @@
         <v>226</v>
       </c>
       <c r="D395" s="6" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E395" s="10">
         <v>93</v>
       </c>
       <c r="F395" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G395" s="6" t="s">
         <v>218</v>
       </c>
       <c r="I395" s="6"/>
       <c r="J395" s="9" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
       <c r="K395" s="6"/>
       <c r="L395" s="12"/>
@@ -21490,7 +21490,7 @@
         <v>341</v>
       </c>
       <c r="R395" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S395"/>
     </row>
@@ -22122,7 +22122,7 @@
         <v>60805</v>
       </c>
       <c r="F413" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G413" s="6" t="s">
         <v>218</v>
@@ -22151,7 +22151,7 @@
         <v>334</v>
       </c>
       <c r="R413" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S413"/>
     </row>
@@ -22172,7 +22172,7 @@
         <v>60677</v>
       </c>
       <c r="F414" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G414" s="6" t="s">
         <v>218</v>
@@ -22201,7 +22201,7 @@
         <v>334</v>
       </c>
       <c r="R414" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S414"/>
     </row>
@@ -22222,7 +22222,7 @@
         <v>52190</v>
       </c>
       <c r="F415" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G415" s="6" t="s">
         <v>218</v>
@@ -22251,7 +22251,7 @@
         <v>334</v>
       </c>
       <c r="R415" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S415"/>
     </row>
@@ -22272,7 +22272,7 @@
         <v>48718</v>
       </c>
       <c r="F416" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G416" s="6" t="s">
         <v>218</v>
@@ -22301,7 +22301,7 @@
         <v>334</v>
       </c>
       <c r="R416" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S416"/>
     </row>
@@ -22322,7 +22322,7 @@
         <v>48649</v>
       </c>
       <c r="F417" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G417" s="6" t="s">
         <v>218</v>
@@ -22351,7 +22351,7 @@
         <v>334</v>
       </c>
       <c r="R417" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S417"/>
     </row>
@@ -22536,7 +22536,7 @@
         <v>41854</v>
       </c>
       <c r="F422" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G422" s="6" t="s">
         <v>218</v>
@@ -22565,7 +22565,7 @@
         <v>334</v>
       </c>
       <c r="R422" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S422"/>
     </row>
@@ -22626,7 +22626,7 @@
         <v>97</v>
       </c>
       <c r="F424" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G424" s="9" t="s">
         <v>218</v>
@@ -22678,7 +22678,7 @@
         <v>97</v>
       </c>
       <c r="F425" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G425" s="9" t="s">
         <v>218</v>
@@ -23152,7 +23152,7 @@
         <v>226</v>
       </c>
       <c r="D437" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G437" s="9" t="s">
         <v>218</v>
@@ -23235,7 +23235,7 @@
         <v>3321</v>
       </c>
       <c r="F439" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G439" s="6" t="s">
         <v>218</v>
@@ -23261,7 +23261,7 @@
         <v>334</v>
       </c>
       <c r="R439" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S439"/>
     </row>
@@ -23282,7 +23282,7 @@
         <v>1915</v>
       </c>
       <c r="F440" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G440" s="6" t="s">
         <v>218</v>
@@ -23308,7 +23308,7 @@
         <v>334</v>
       </c>
       <c r="R440" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S440"/>
     </row>
@@ -23497,7 +23497,7 @@
         <v>15050</v>
       </c>
       <c r="F445" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G445" s="6" t="s">
         <v>218</v>
@@ -23523,7 +23523,7 @@
         <v>171</v>
       </c>
       <c r="R445" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S445"/>
     </row>
@@ -23538,7 +23538,7 @@
         <v>226</v>
       </c>
       <c r="D446" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G446" s="9" t="s">
         <v>218</v>
@@ -23578,13 +23578,13 @@
         <v>226</v>
       </c>
       <c r="D447" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E447" s="10">
         <v>21</v>
       </c>
       <c r="F447" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G447" s="9" t="s">
         <v>218</v>
@@ -23785,7 +23785,7 @@
         <v>1789</v>
       </c>
       <c r="F453" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G453" s="6" t="s">
         <v>218</v>
@@ -23811,7 +23811,7 @@
         <v>334</v>
       </c>
       <c r="R453" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S453"/>
     </row>
@@ -23916,7 +23916,7 @@
         <v>2043</v>
       </c>
       <c r="F456" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G456" s="6" t="s">
         <v>218</v>
@@ -23942,7 +23942,7 @@
         <v>334</v>
       </c>
       <c r="R456" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S456"/>
     </row>
@@ -24066,7 +24066,7 @@
     </row>
     <row r="460" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A460" s="6" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
       <c r="B460" s="9" t="s">
         <v>293</v>
@@ -24093,7 +24093,7 @@
         <v>0</v>
       </c>
       <c r="O460" s="6" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="P460" s="9" t="s">
         <v>323</v>
@@ -24102,7 +24102,7 @@
         <v>171</v>
       </c>
       <c r="R460" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S460"/>
     </row>
@@ -24123,7 +24123,7 @@
         <v>1812</v>
       </c>
       <c r="F461" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G461" s="6" t="s">
         <v>218</v>
@@ -24149,13 +24149,13 @@
         <v>334</v>
       </c>
       <c r="R461" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S461"/>
     </row>
     <row r="462" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A462" s="6" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
       <c r="B462" s="9" t="s">
         <v>293</v>
@@ -24182,7 +24182,7 @@
         <v>0</v>
       </c>
       <c r="O462" s="6" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="P462" s="9" t="s">
         <v>323</v>
@@ -24191,7 +24191,7 @@
         <v>171</v>
       </c>
       <c r="R462" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S462"/>
     </row>
@@ -24286,7 +24286,7 @@
         <v>65</v>
       </c>
       <c r="F465" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G465" s="9" t="s">
         <v>218</v>
@@ -24352,7 +24352,7 @@
         <v>15240</v>
       </c>
       <c r="F467" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G467" s="6" t="s">
         <v>218</v>
@@ -24380,7 +24380,7 @@
         <v>334</v>
       </c>
       <c r="R467" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S467"/>
     </row>
@@ -24531,7 +24531,7 @@
         <v>15240</v>
       </c>
       <c r="F472" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G472" s="6" t="s">
         <v>218</v>
@@ -24559,7 +24559,7 @@
         <v>334</v>
       </c>
       <c r="R472" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S472"/>
     </row>
@@ -24716,7 +24716,7 @@
         <v>15237</v>
       </c>
       <c r="F477" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G477" s="6" t="s">
         <v>218</v>
@@ -24744,7 +24744,7 @@
         <v>334</v>
       </c>
       <c r="R477" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S477"/>
     </row>
@@ -24765,7 +24765,7 @@
         <v>14537</v>
       </c>
       <c r="F478" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G478" s="6" t="s">
         <v>218</v>
@@ -24793,7 +24793,7 @@
         <v>334</v>
       </c>
       <c r="R478" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S478"/>
     </row>
@@ -24814,7 +24814,7 @@
         <v>15239</v>
       </c>
       <c r="F479" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G479" s="6" t="s">
         <v>218</v>
@@ -24842,7 +24842,7 @@
         <v>334</v>
       </c>
       <c r="R479" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S479"/>
     </row>
@@ -24863,7 +24863,7 @@
         <v>15236</v>
       </c>
       <c r="F480" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G480" s="6" t="s">
         <v>218</v>
@@ -24891,7 +24891,7 @@
         <v>334</v>
       </c>
       <c r="R480" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S480"/>
     </row>
@@ -24906,25 +24906,25 @@
         <v>226</v>
       </c>
       <c r="D481" s="6" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="E481" s="10">
         <v>117</v>
       </c>
       <c r="F481" s="10" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="G481" s="6" t="s">
         <v>218</v>
       </c>
       <c r="H481" s="7" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
       <c r="I481" s="9" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
       <c r="J481" s="9" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="K481" s="6"/>
       <c r="L481" s="12"/>
@@ -24941,7 +24941,7 @@
         <v>334</v>
       </c>
       <c r="R481" s="15" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="482" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
@@ -25657,7 +25657,7 @@
         <v>226</v>
       </c>
       <c r="D506" s="9" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="G506" s="9" t="s">
         <v>218</v>
@@ -26133,7 +26133,7 @@
     </row>
     <row r="518" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A518" s="6" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="B518" s="9" t="s">
         <v>293</v>
@@ -26160,7 +26160,7 @@
         <v>0</v>
       </c>
       <c r="O518" s="6" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="P518" s="9" t="s">
         <v>323</v>
@@ -26169,7 +26169,7 @@
         <v>341</v>
       </c>
       <c r="R518" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S518"/>
     </row>
@@ -26273,7 +26273,7 @@
         <v>1677</v>
       </c>
       <c r="F521" s="10" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="G521" s="6" t="s">
         <v>218</v>
@@ -26298,7 +26298,7 @@
         <v>334</v>
       </c>
       <c r="R521" s="2" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="S521"/>
     </row>
@@ -26397,13 +26397,13 @@
         <v>1334</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G1" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -26417,7 +26417,7 @@
         <v>1335</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E2" t="s">
         <v>219</v>
@@ -26426,7 +26426,7 @@
         <v>219</v>
       </c>
       <c r="G2" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -26440,7 +26440,7 @@
         <v>1336</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="E3" t="s">
         <v>243</v>
@@ -26449,7 +26449,7 @@
         <v>243</v>
       </c>
       <c r="G3" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -26463,7 +26463,7 @@
         <v>1335</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="E4" t="s">
         <v>243</v>
@@ -26472,7 +26472,7 @@
         <v>219</v>
       </c>
       <c r="G4" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -26486,7 +26486,7 @@
         <v>1336</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E5" t="s">
         <v>219</v>
@@ -26495,7 +26495,7 @@
         <v>243</v>
       </c>
       <c r="G5" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -26506,10 +26506,10 @@
         <v>1350</v>
       </c>
       <c r="C6" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>243</v>
@@ -26529,13 +26529,13 @@
         <v>1337</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G7" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -26546,10 +26546,10 @@
         <v>1351</v>
       </c>
       <c r="C8" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="E8" t="s">
         <v>219</v>
@@ -26558,7 +26558,7 @@
         <v>219</v>
       </c>
       <c r="G8" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -26569,10 +26569,10 @@
         <v>1351</v>
       </c>
       <c r="C9" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="E9" t="s">
         <v>243</v>
@@ -26581,7 +26581,7 @@
         <v>243</v>
       </c>
       <c r="G9" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -26592,10 +26592,10 @@
         <v>1351</v>
       </c>
       <c r="C10" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="E10" t="s">
         <v>219</v>
@@ -26604,7 +26604,7 @@
         <v>243</v>
       </c>
       <c r="G10" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -26615,10 +26615,10 @@
         <v>1351</v>
       </c>
       <c r="C11" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="E11" t="s">
         <v>243</v>
@@ -26627,7 +26627,7 @@
         <v>219</v>
       </c>
       <c r="G11" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -26641,7 +26641,7 @@
         <v>1338</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="E12" t="s">
         <v>219</v>
@@ -26650,7 +26650,7 @@
         <v>219</v>
       </c>
       <c r="G12" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -26664,7 +26664,7 @@
         <v>1339</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="E13" t="s">
         <v>243</v>
@@ -26687,7 +26687,7 @@
         <v>1339</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="E14" t="s">
         <v>219</v>
@@ -26710,7 +26710,7 @@
         <v>1338</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="E15" t="s">
         <v>243</v>
@@ -26719,7 +26719,7 @@
         <v>219</v>
       </c>
       <c r="G15" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -26733,13 +26733,13 @@
         <v>1341</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G16" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -26750,10 +26750,10 @@
         <v>1353</v>
       </c>
       <c r="C17" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>243</v>
@@ -26773,13 +26773,13 @@
         <v>1342</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G18" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -26790,16 +26790,16 @@
         <v>1354</v>
       </c>
       <c r="C19" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>243</v>
       </c>
       <c r="G19" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -26813,7 +26813,7 @@
         <v>1343</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="E20" t="s">
         <v>219</v>
@@ -26822,7 +26822,7 @@
         <v>219</v>
       </c>
       <c r="G20" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -26836,7 +26836,7 @@
         <v>1344</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="E21" t="s">
         <v>219</v>
@@ -26845,7 +26845,7 @@
         <v>219</v>
       </c>
       <c r="G21" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -26859,7 +26859,7 @@
         <v>1345</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="E22" t="s">
         <v>219</v>
@@ -26868,7 +26868,7 @@
         <v>219</v>
       </c>
       <c r="G22" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -26882,7 +26882,7 @@
         <v>1346</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="E23" t="s">
         <v>243</v>
@@ -26891,7 +26891,7 @@
         <v>243</v>
       </c>
       <c r="G23" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -26905,7 +26905,7 @@
         <v>1346</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="E24" t="s">
         <v>219</v>
@@ -26914,7 +26914,7 @@
         <v>243</v>
       </c>
       <c r="G24" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -26928,7 +26928,7 @@
         <v>1345</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="E25" t="s">
         <v>243</v>
@@ -26937,7 +26937,7 @@
         <v>219</v>
       </c>
       <c r="G25" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -26951,13 +26951,13 @@
         <v>1340</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G26" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -26971,13 +26971,13 @@
         <v>1347</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G27" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -26988,16 +26988,16 @@
         <v>1359</v>
       </c>
       <c r="C28" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>243</v>
       </c>
       <c r="G28" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -27005,20 +27005,20 @@
         <v>50</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="C29" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="11" t="s">
         <v>243</v>
       </c>
       <c r="G29" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="9"/>
@@ -27029,20 +27029,20 @@
         <v>50</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="C30" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="11" t="s">
         <v>219</v>
       </c>
       <c r="G30" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="9"/>
@@ -27053,20 +27053,20 @@
         <v>72</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="C31" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="11" t="s">
         <v>243</v>
       </c>
       <c r="G31" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="9"/>
@@ -27077,20 +27077,20 @@
         <v>184</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C32" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="11" t="s">
         <v>219</v>
       </c>
       <c r="G32" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="9"/>
@@ -27101,20 +27101,20 @@
         <v>184</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C33" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="11" t="s">
         <v>243</v>
       </c>
       <c r="G33" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="9"/>

</xml_diff>